<commit_message>
Update on 20200410 part 3
</commit_message>
<xml_diff>
--- a/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200409/宽带IPOE通道子产品配置(206295976)/宽带IPOE通道子产品配置(206295976)测试报告.xlsx
+++ b/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200409/宽带IPOE通道子产品配置(206295976)/宽带IPOE通道子产品配置(206295976)测试报告.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>序号</t>
   </si>
@@ -335,8 +335,12 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>新CRM反馈规则引擎尚未开发完成,需要延期</t>
+    <t xml:space="preserve">该场景新CRM反馈cpc先上，规则此版本不上仿真，会在之后版本迭代
+</t>
     <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>该场景新CRM反馈cpc先上，规则此版本不上仿真，会在之后版本迭代</t>
   </si>
 </sst>
 </file>
@@ -512,17 +516,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,9 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
   <cols>
@@ -1137,38 +1139,38 @@
         <v>45</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="24">
         <v>4</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="23">
+      <c r="K2" s="26">
         <v>206295976</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="23" t="s">
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="23"/>
+      <c r="S2" s="26"/>
       <c r="T2" s="21"/>
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
@@ -1418,20 +1420,20 @@
         <v>46</v>
       </c>
       <c r="E3" s="14"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
       <c r="T3" s="21"/>
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
@@ -1667,7 +1669,7 @@
       <c r="IR3" s="21"/>
       <c r="IS3" s="21"/>
     </row>
-    <row r="4" spans="1:253" ht="48">
+    <row r="4" spans="1:253" ht="84">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -1683,20 +1685,20 @@
       <c r="E4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21"/>
       <c r="V4" s="21"/>
@@ -1946,20 +1948,20 @@
         <v>47</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
       <c r="T5" s="21"/>
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
@@ -2197,20 +2199,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="Q2:Q5"/>
+    <mergeCell ref="R2:R5"/>
+    <mergeCell ref="S2:S5"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="N2:N5"/>
+    <mergeCell ref="O2:O5"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="I2:I5"/>
     <mergeCell ref="J2:J5"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="N2:N5"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="Q2:Q5"/>
-    <mergeCell ref="R2:R5"/>
-    <mergeCell ref="S2:S5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2300,7 +2302,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51">
+    <row r="3" spans="1:10" ht="72">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -2323,7 +2325,7 @@
         <v>52</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="3" t="s">

</xml_diff>

<commit_message>
Update on 20200410 part 4
</commit_message>
<xml_diff>
--- a/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200409/宽带IPOE通道子产品配置(206295976)/宽带IPOE通道子产品配置(206295976)测试报告.xlsx
+++ b/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200409/宽带IPOE通道子产品配置(206295976)/宽带IPOE通道子产品配置(206295976)测试报告.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="测试概况" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>序号</t>
   </si>
@@ -335,12 +335,8 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">该场景新CRM反馈cpc先上，规则此版本不上仿真，会在之后版本迭代
-</t>
+    <t>需求内提到IPOE通道子产品是面向500M及以下宽带,该场景新CRM规则引擎因为未能开发完成,故此版本不上仿真,会在之后版本后续迭代</t>
     <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>该场景新CRM反馈cpc先上，规则此版本不上仿真，会在之后版本迭代</t>
   </si>
 </sst>
 </file>
@@ -516,17 +512,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
   <cols>
@@ -1139,38 +1135,38 @@
         <v>45</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="26">
         <v>4</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="24">
         <v>206295976</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26" t="s">
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="26"/>
+      <c r="S2" s="24"/>
       <c r="T2" s="21"/>
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
@@ -1420,20 +1416,20 @@
         <v>46</v>
       </c>
       <c r="E3" s="14"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
       <c r="T3" s="21"/>
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
@@ -1669,7 +1665,7 @@
       <c r="IR3" s="21"/>
       <c r="IS3" s="21"/>
     </row>
-    <row r="4" spans="1:253" ht="84">
+    <row r="4" spans="1:253" ht="132">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -1685,20 +1681,20 @@
       <c r="E4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21"/>
       <c r="V4" s="21"/>
@@ -1948,20 +1944,20 @@
         <v>47</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
       <c r="T5" s="21"/>
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
@@ -2199,6 +2195,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="J2:J5"/>
     <mergeCell ref="P2:P5"/>
     <mergeCell ref="Q2:Q5"/>
     <mergeCell ref="R2:R5"/>
@@ -2208,11 +2209,6 @@
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="N2:N5"/>
     <mergeCell ref="O2:O5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="J2:J5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2223,7 +2219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
   <cols>
@@ -2302,7 +2298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="72">
+    <row r="3" spans="1:10" ht="132">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -2325,7 +2321,7 @@
         <v>52</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="3" t="s">

</xml_diff>